<commit_message>
1) used picante package to calc phylogenetic distance (PD), species richness (SR), and families (Fam) represented by each Urban Tolerance Index (UAI, MUTI, and UN). 2) also, began to use picante package to caluclate phylogenetic signal of predictor traits (using group rds files)
</commit_message>
<xml_diff>
--- a/Notes/Coastal_Sample_Size_Corr.xlsx
+++ b/Notes/Coastal_Sample_Size_Corr.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA28A631-60FC-4EB9-86E7-EB4240FF06E8}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B21B837-877A-4524-A128-3AE022CAC933}"/>
   <bookViews>
-    <workbookView xWindow="10010" yWindow="310" windowWidth="9260" windowHeight="11200" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -511,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -534,109 +533,108 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,6 +651,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,8 +977,8 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,7 +1020,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="42" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1027,51 +1029,51 @@
       <c r="C2" s="3">
         <v>237</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="9"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>69</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="K3" s="12" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7">
         <v>38</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="K4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="15">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="K4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="11">
         <v>798</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1080,92 +1082,92 @@
       <c r="C5" s="3">
         <v>202</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
       <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="12">
         <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5">
         <v>68</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="K6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="18">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="K6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="14">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="7">
         <v>129</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="11">
         <v>798</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>130</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <v>129</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1174,39 +1176,39 @@
       <c r="C11" s="3">
         <v>796</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="9"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>130</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="10"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="7">
         <v>129</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:12" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1215,39 +1217,39 @@
       <c r="C14" s="3">
         <v>738</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5">
         <v>126</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="7">
         <v>122</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1256,53 +1258,53 @@
       <c r="C17" s="3">
         <v>408</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="15">
         <v>421</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <v>345</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="9"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5">
         <v>121</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="20">
+      <c r="D18" s="35"/>
+      <c r="E18" s="16">
         <v>73</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="16">
         <v>54</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="10"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7">
         <v>102</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="21">
+      <c r="D19" s="36"/>
+      <c r="E19" s="17">
         <v>97</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="17">
         <v>32</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1311,7 +1313,7 @@
       <c r="C20" s="3">
         <v>766</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="32" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="3">
@@ -1320,47 +1322,47 @@
       <c r="F20" s="3">
         <v>615</v>
       </c>
-      <c r="G20" s="22"/>
+      <c r="G20" s="18"/>
       <c r="I20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="9"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>127</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="5">
         <v>10</v>
       </c>
       <c r="F21" s="5">
         <v>107</v>
       </c>
-      <c r="G21" s="22"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="7">
         <v>129</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="7">
         <v>8</v>
       </c>
       <c r="F22" s="7">
         <v>114</v>
       </c>
-      <c r="G22" s="22"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1370,7 +1372,7 @@
         <f>E20+F20</f>
         <v>733</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="37" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="3">
@@ -1379,54 +1381,54 @@
       <c r="F23" s="3">
         <v>507</v>
       </c>
-      <c r="G23" s="22"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="9"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>117</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="5">
         <v>55</v>
       </c>
       <c r="F24" s="5">
         <v>75</v>
       </c>
-      <c r="G24" s="22"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="10"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="7">
         <v>122</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="7">
         <v>79</v>
       </c>
       <c r="F25" s="7">
         <v>50</v>
       </c>
-      <c r="G25" s="22"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3">
-        <f>E23+F23</f>
+        <f t="shared" ref="C26:C31" si="0">E23+F23</f>
         <v>796</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="37" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="3">
@@ -1435,131 +1437,131 @@
       <c r="F26" s="3">
         <v>506</v>
       </c>
-      <c r="G26" s="22"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="9"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="5">
-        <f>E24+F24</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="D27" s="26"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="5">
         <v>36</v>
       </c>
       <c r="F27" s="5">
         <v>94</v>
       </c>
-      <c r="G27" s="22"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="7">
-        <f>E25+F25</f>
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="7">
         <v>25</v>
       </c>
       <c r="F28" s="7">
         <v>104</v>
       </c>
-      <c r="G28" s="22"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="38" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3">
-        <f>E26+F26</f>
+        <f t="shared" si="0"/>
         <v>796</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="9"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="5">
-        <f>E27+F27</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="10"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="7">
-        <f>E28+F28</f>
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="11">
         <v>766</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="9"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="12">
         <v>127</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="10"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="14">
         <v>129</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1568,91 +1570,91 @@
       <c r="C35" s="3">
         <v>766</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="9"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="5">
         <v>127</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="10"/>
-      <c r="B37" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="33">
+      <c r="A37" s="40"/>
+      <c r="B37" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="22">
         <v>129</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="31">
+      <c r="B38" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="20">
         <v>766</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="9"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="5">
         <v>127</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="10"/>
-      <c r="B40" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="33">
+      <c r="A40" s="40"/>
+      <c r="B40" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="22">
         <v>129</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="31">
+      <c r="B41" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="20">
         <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="9"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
@@ -1661,73 +1663,69 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="10"/>
-      <c r="B43" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="33">
+      <c r="A43" s="40"/>
+      <c r="B43" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="22">
         <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="31">
+      <c r="B44" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="20">
         <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="9"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="5">
         <v>67</v>
       </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="10"/>
-      <c r="B46" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="33">
+      <c r="A46" s="40"/>
+      <c r="B46" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="22">
         <v>61</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="31">
+      <c r="B47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="20">
         <f>E47+F47</f>
         <v>766</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E47" s="31">
+      <c r="E47" s="20">
         <v>735</v>
       </c>
-      <c r="F47" s="31">
+      <c r="F47" s="20">
         <v>31</v>
       </c>
-      <c r="G47" s="35"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="9"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="4" t="s">
         <v>11</v>
       </c>
@@ -1735,58 +1733,57 @@
         <f>127</f>
         <v>127</v>
       </c>
-      <c r="D48" s="29"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="5">
         <v>121</v>
       </c>
       <c r="F48" s="5">
         <v>6</v>
       </c>
-      <c r="G48" s="35"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="10"/>
-      <c r="B49" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="33">
+      <c r="A49" s="40"/>
+      <c r="B49" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="22">
         <v>129</v>
       </c>
-      <c r="D49" s="36"/>
-      <c r="E49" s="33">
+      <c r="D49" s="28"/>
+      <c r="E49" s="22">
         <v>121</v>
       </c>
-      <c r="F49" s="33">
+      <c r="F49" s="22">
         <v>8</v>
       </c>
-      <c r="G49" s="34"/>
+      <c r="G49" s="23"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="31" t="e" cm="1">
+      <c r="B50" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="20" t="e" cm="1">
         <f t="array" ref="C50">E50+E55F50+G50</f>
         <v>#NAME?</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="31">
+      <c r="E50" s="20">
         <v>405</v>
       </c>
-      <c r="F50" s="31">
+      <c r="F50" s="20">
         <v>290</v>
       </c>
-      <c r="G50" s="31">
+      <c r="G50" s="20">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="9"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="4" t="s">
         <v>11</v>
       </c>
@@ -1794,7 +1791,7 @@
         <f>E51+F51+G51</f>
         <v>127</v>
       </c>
-      <c r="D51" s="39"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="5">
         <v>68</v>
       </c>
@@ -1806,70 +1803,70 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="10"/>
-      <c r="B52" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="33">
+      <c r="A52" s="40"/>
+      <c r="B52" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="22">
         <f>E52+F52+G52</f>
         <v>129</v>
       </c>
-      <c r="D52" s="40"/>
-      <c r="E52" s="33">
+      <c r="D52" s="31"/>
+      <c r="E52" s="22">
         <v>57</v>
       </c>
-      <c r="F52" s="33">
+      <c r="F52" s="22">
         <v>65</v>
       </c>
-      <c r="G52" s="33">
+      <c r="G52" s="22">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="15">
+      <c r="B53" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="11">
         <v>798</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="9"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="12">
         <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="37"/>
-      <c r="B55" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="18">
+      <c r="A55" s="41"/>
+      <c r="B55" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="14">
         <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D56" s="41"/>
+      <c r="D56" s="24"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D57" s="42"/>
+      <c r="D57" s="25"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D58" s="43"/>
+      <c r="D58" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="A8:A10"/>
@@ -1883,27 +1880,13 @@
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A32:A34"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D23:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326BD05C-C400-47D5-890C-E6753065AEDC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
removed territoriality = 2 from MUTI and UN models. re-ran without territoriality = 2.
</commit_message>
<xml_diff>
--- a/Notes/Coastal_Sample_Size_Corr.xlsx
+++ b/Notes/Coastal_Sample_Size_Corr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B21B837-877A-4524-A128-3AE022CAC933}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9DB794-50C7-4403-8FEA-D109CE9D275E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
   </bookViews>
@@ -175,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -510,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -560,9 +574,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -588,6 +599,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -612,29 +644,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,8 +1018,8 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,7 +1061,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1029,23 +1070,23 @@
       <c r="C2" s="3">
         <v>237</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="39"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>69</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
       <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1054,17 +1095,17 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="40"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7">
         <v>38</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1073,7 +1114,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1082,10 +1123,10 @@
       <c r="C5" s="3">
         <v>202</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
       <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1094,17 +1135,17 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="39"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5">
         <v>68</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
       <c r="K6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1113,20 +1154,20 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="7">
         <v>129</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="29" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1135,39 +1176,39 @@
       <c r="C8" s="11">
         <v>798</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="39"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="12">
         <v>130</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="40"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="14">
         <v>129</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1176,39 +1217,39 @@
       <c r="C11" s="3">
         <v>796</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="39"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>130</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="40"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="7">
         <v>129</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:12" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1217,39 +1258,39 @@
       <c r="C14" s="3">
         <v>738</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="39"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5">
         <v>126</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="40"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="7">
         <v>122</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1258,53 +1299,41 @@
       <c r="C17" s="3">
         <v>408</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="15">
-        <v>421</v>
-      </c>
-      <c r="F17" s="15">
-        <v>345</v>
-      </c>
-      <c r="G17" s="18"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="39"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5">
         <v>121</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="16">
-        <v>73</v>
-      </c>
-      <c r="F18" s="16">
-        <v>54</v>
-      </c>
-      <c r="G18" s="18"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="40"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7">
         <v>102</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="17">
-        <v>97</v>
-      </c>
-      <c r="F19" s="17">
-        <v>32</v>
-      </c>
-      <c r="G19" s="18"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1313,56 +1342,56 @@
       <c r="C20" s="3">
         <v>766</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="3">
-        <v>118</v>
-      </c>
-      <c r="F20" s="3">
-        <v>615</v>
-      </c>
-      <c r="G20" s="18"/>
+      <c r="E20" s="15">
+        <v>421</v>
+      </c>
+      <c r="F20" s="15">
+        <v>345</v>
+      </c>
+      <c r="G20" s="17"/>
       <c r="I20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="39"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>127</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="5">
-        <v>10</v>
-      </c>
-      <c r="F21" s="5">
-        <v>107</v>
-      </c>
-      <c r="G21" s="18"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="16">
+        <v>73</v>
+      </c>
+      <c r="F21" s="16">
+        <v>54</v>
+      </c>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="40"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="7">
         <v>129</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="7">
-        <v>8</v>
-      </c>
-      <c r="F22" s="7">
-        <v>114</v>
-      </c>
-      <c r="G22" s="18"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="46">
+        <v>97</v>
+      </c>
+      <c r="F22" s="47">
+        <v>32</v>
+      </c>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1370,55 +1399,55 @@
       </c>
       <c r="C23" s="3">
         <f>E20+F20</f>
-        <v>733</v>
-      </c>
-      <c r="D23" s="37" t="s">
+        <v>766</v>
+      </c>
+      <c r="D23" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="3">
-        <v>289</v>
-      </c>
-      <c r="F23" s="3">
-        <v>507</v>
-      </c>
-      <c r="G23" s="18"/>
+      <c r="E23" s="19">
+        <v>118</v>
+      </c>
+      <c r="F23" s="19">
+        <v>615</v>
+      </c>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="39"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>117</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="5">
-        <v>55</v>
+      <c r="D24" s="31"/>
+      <c r="E24" s="48">
+        <v>10</v>
       </c>
       <c r="F24" s="5">
-        <v>75</v>
-      </c>
-      <c r="G24" s="18"/>
+        <v>107</v>
+      </c>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="40"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="44">
         <v>122</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="7">
-        <v>79</v>
-      </c>
-      <c r="F25" s="7">
-        <v>50</v>
-      </c>
-      <c r="G25" s="18"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="44">
+        <v>8</v>
+      </c>
+      <c r="F25" s="44">
+        <v>114</v>
+      </c>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1426,57 +1455,57 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" ref="C26:C31" si="0">E23+F23</f>
-        <v>796</v>
-      </c>
-      <c r="D26" s="37" t="s">
+        <v>733</v>
+      </c>
+      <c r="D26" s="30" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="3">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F26" s="3">
-        <v>506</v>
-      </c>
-      <c r="G26" s="18"/>
+        <v>507</v>
+      </c>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="39"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="D27" s="35"/>
+        <v>117</v>
+      </c>
+      <c r="D27" s="31"/>
       <c r="E27" s="5">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F27" s="5">
-        <v>94</v>
-      </c>
-      <c r="G27" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="40"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="7">
         <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-      <c r="D28" s="35"/>
+        <v>122</v>
+      </c>
+      <c r="D28" s="31"/>
       <c r="E28" s="7">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="F28" s="7">
-        <v>104</v>
-      </c>
-      <c r="G28" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1486,13 +1515,17 @@
         <f t="shared" si="0"/>
         <v>796</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="3">
+        <v>290</v>
+      </c>
+      <c r="F29" s="3">
+        <v>506</v>
+      </c>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="39"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1500,13 +1533,17 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="5">
+        <v>36</v>
+      </c>
+      <c r="F30" s="5">
+        <v>94</v>
+      </c>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="40"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
@@ -1514,13 +1551,17 @@
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="7">
+        <v>25</v>
+      </c>
+      <c r="F31" s="7">
+        <v>104</v>
+      </c>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1529,39 +1570,39 @@
       <c r="C32" s="11">
         <v>766</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="39"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="12">
         <v>127</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="40"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="14">
         <v>129</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="29" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1570,91 +1611,91 @@
       <c r="C35" s="3">
         <v>766</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="39"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="5">
         <v>127</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="40"/>
-      <c r="B37" s="21" t="s">
+      <c r="A37" s="28"/>
+      <c r="B37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="21">
         <v>129</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="19">
         <v>766</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="39"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="5">
         <v>127</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="40"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="28"/>
+      <c r="B40" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="21">
         <v>129</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="19">
         <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="39"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
@@ -1663,27 +1704,27 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="40"/>
-      <c r="B43" s="21" t="s">
+      <c r="A43" s="28"/>
+      <c r="B43" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="21">
         <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="19">
         <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="39"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
@@ -1692,98 +1733,98 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="40"/>
-      <c r="B46" s="21" t="s">
+      <c r="A46" s="28"/>
+      <c r="B46" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="21">
         <v>61</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="19">
         <f>E47+F47</f>
         <v>766</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="19">
         <v>735</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="19">
         <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="39"/>
-      <c r="B48" s="4" t="s">
+      <c r="A48" s="27"/>
+      <c r="B48" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="42">
         <f>127</f>
         <v>127</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="5">
+      <c r="D48" s="33"/>
+      <c r="E48" s="42">
         <v>121</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="42">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="40"/>
-      <c r="B49" s="21" t="s">
+      <c r="A49" s="28"/>
+      <c r="B49" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="43">
         <v>129</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="22">
+      <c r="D49" s="34"/>
+      <c r="E49" s="43">
         <v>121</v>
       </c>
-      <c r="F49" s="22">
+      <c r="F49" s="43">
         <v>8</v>
       </c>
-      <c r="G49" s="23"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="20" t="e" cm="1">
+      <c r="C50" s="19" t="e" cm="1">
         <f t="array" ref="C50">E50+E55F50+G50</f>
         <v>#NAME?</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="19">
         <v>405</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="19">
         <v>290</v>
       </c>
-      <c r="G50" s="20">
+      <c r="G50" s="19">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="39"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="4" t="s">
         <v>11</v>
       </c>
@@ -1791,42 +1832,42 @@
         <f>E51+F51+G51</f>
         <v>127</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="36"/>
       <c r="E51" s="5">
         <v>68</v>
       </c>
       <c r="F51" s="5">
         <v>55</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="40"/>
-      <c r="B52" s="21" t="s">
+      <c r="A52" s="28"/>
+      <c r="B52" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="22">
+      <c r="C52" s="21">
         <f>E52+F52+G52</f>
         <v>129</v>
       </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="22">
+      <c r="D52" s="37"/>
+      <c r="E52" s="21">
         <v>57</v>
       </c>
-      <c r="F52" s="22">
+      <c r="F52" s="21">
         <v>65</v>
       </c>
-      <c r="G52" s="22">
+      <c r="G52" s="43">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="11">
@@ -1834,7 +1875,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="39"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="4" t="s">
         <v>11</v>
       </c>
@@ -1843,8 +1884,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="41"/>
-      <c r="B55" s="21" t="s">
+      <c r="A55" s="32"/>
+      <c r="B55" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="14">
@@ -1852,21 +1893,19 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D56" s="24"/>
+      <c r="D56" s="23"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D57" s="25"/>
+      <c r="D57" s="24"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D58" s="26"/>
+      <c r="D58" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D23:D25"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="A8:A10"/>
@@ -1883,10 +1922,13 @@
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
found total (across all indexes) sample sizes for predictor traits. I wanted this information for our methods section.
</commit_message>
<xml_diff>
--- a/Notes/Coastal_Sample_Size_Corr.xlsx
+++ b/Notes/Coastal_Sample_Size_Corr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9DB794-50C7-4403-8FEA-D109CE9D275E}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{254FBCFA-0BA0-4808-B627-D30555D4B8E4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,28 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
@@ -175,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +188,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -237,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -520,9 +506,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -599,87 +597,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1017,9 +1016,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1970122C-29C4-4E46-A235-3E0E6C7793EA}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1031,7 +1030,7 @@
     <col min="12" max="12" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="53" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="40" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1060,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1074,9 +1073,12 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
+      <c r="H2" s="51">
+        <v>237</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="27"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1087,6 +1089,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
+      <c r="H3" s="51"/>
       <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1095,7 +1098,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1106,6 +1109,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
+      <c r="H4" s="51"/>
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1118,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1127,6 +1131,9 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
+      <c r="H5" s="51">
+        <v>210</v>
+      </c>
       <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1135,7 +1142,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="27"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1146,6 +1153,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
+      <c r="H6" s="51"/>
       <c r="K6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1162,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="28"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1165,9 +1173,10 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
+      <c r="H7" s="51"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="41" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1180,9 +1189,12 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
+      <c r="H8" s="51">
+        <v>807</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="27"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1193,9 +1205,10 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="28"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1206,9 +1219,10 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1221,9 +1235,12 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
+      <c r="H11" s="51">
+        <v>805</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="27"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1234,9 +1251,10 @@
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
+      <c r="H12" s="51"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="28"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
@@ -1247,9 +1265,10 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
+      <c r="H13" s="51"/>
     </row>
     <row r="14" spans="1:12" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1262,9 +1281,12 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
+      <c r="H14" s="51">
+        <v>746</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="27"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1275,9 +1297,10 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
+      <c r="H15" s="51"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="28"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1288,9 +1311,10 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
+      <c r="H16" s="51"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1299,41 +1323,46 @@
       <c r="C17" s="3">
         <v>408</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="17"/>
+      <c r="H17" s="51">
+        <v>484</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5">
         <v>121</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="17"/>
+      <c r="H18" s="51"/>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="28"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7">
         <v>102</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="17"/>
+      <c r="H19" s="51"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1342,7 +1371,7 @@
       <c r="C20" s="3">
         <v>766</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="15">
@@ -1352,19 +1381,22 @@
         <v>345</v>
       </c>
       <c r="G20" s="17"/>
+      <c r="H20" s="51">
+        <v>775</v>
+      </c>
       <c r="I20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>127</v>
       </c>
-      <c r="D21" s="39"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="16">
         <v>73</v>
       </c>
@@ -1372,26 +1404,28 @@
         <v>54</v>
       </c>
       <c r="G21" s="17"/>
+      <c r="H21" s="51"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="28"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="7">
         <v>129</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="46">
+      <c r="D22" s="37"/>
+      <c r="E22" s="29">
         <v>97</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="30">
         <v>32</v>
       </c>
       <c r="G22" s="17"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1401,7 +1435,7 @@
         <f>E20+F20</f>
         <v>766</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="40" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="19">
@@ -1411,43 +1445,48 @@
         <v>615</v>
       </c>
       <c r="G23" s="17"/>
+      <c r="H23" s="51">
+        <v>741</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>117</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="48">
+      <c r="D24" s="38"/>
+      <c r="E24" s="31">
         <v>10</v>
       </c>
       <c r="F24" s="5">
         <v>107</v>
       </c>
       <c r="G24" s="17"/>
+      <c r="H24" s="51"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="28"/>
-      <c r="B25" s="51" t="s">
+      <c r="A25" s="43"/>
+      <c r="B25" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="28">
         <v>122</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="44">
+      <c r="D25" s="38"/>
+      <c r="E25" s="28">
         <v>8</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="28">
         <v>114</v>
       </c>
       <c r="G25" s="17"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="41" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1457,7 +1496,7 @@
         <f t="shared" ref="C26:C31" si="0">E23+F23</f>
         <v>733</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="40" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="3">
@@ -1467,9 +1506,12 @@
         <v>507</v>
       </c>
       <c r="G26" s="17"/>
+      <c r="H26" s="51">
+        <v>805</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="27"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1519,7 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="5">
         <v>55</v>
       </c>
@@ -1485,9 +1527,10 @@
         <v>75</v>
       </c>
       <c r="G27" s="17"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="28"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="6" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1538,7 @@
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="D28" s="31"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="7">
         <v>79</v>
       </c>
@@ -1503,9 +1546,10 @@
         <v>50</v>
       </c>
       <c r="G28" s="17"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1523,9 +1567,12 @@
         <v>506</v>
       </c>
       <c r="G29" s="17"/>
+      <c r="H29" s="51">
+        <v>805</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="27"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1541,9 +1588,10 @@
         <v>94</v>
       </c>
       <c r="G30" s="17"/>
+      <c r="H30" s="51"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="28"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
@@ -1559,9 +1607,10 @@
         <v>104</v>
       </c>
       <c r="G31" s="17"/>
+      <c r="H31" s="51"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1574,9 +1623,12 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="27"/>
+      <c r="H32" s="51">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="42"/>
       <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
@@ -1587,9 +1639,10 @@
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="28"/>
+      <c r="H33" s="51"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="43"/>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
@@ -1600,9 +1653,10 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="29" t="s">
+      <c r="H34" s="51"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1615,9 +1669,12 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="27"/>
+      <c r="H35" s="51">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="42"/>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
@@ -1628,9 +1685,10 @@
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="28"/>
+      <c r="H36" s="51"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="43"/>
       <c r="B37" s="20" t="s">
         <v>7</v>
       </c>
@@ -1641,9 +1699,10 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="29" t="s">
+      <c r="H37" s="51"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -1656,9 +1715,12 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="27"/>
+      <c r="H38" s="51">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="42"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1669,9 +1731,10 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="28"/>
+      <c r="H39" s="51"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="43"/>
       <c r="B40" s="20" t="s">
         <v>7</v>
       </c>
@@ -1682,9 +1745,10 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="29" t="s">
+      <c r="H40" s="51"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="18" t="s">
@@ -1693,27 +1757,32 @@
       <c r="C41" s="19">
         <v>201</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="27"/>
+      <c r="H41" s="51">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="42"/>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="5">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="28"/>
+      <c r="H42" s="51"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="43"/>
       <c r="B43" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="21">
         <v>61</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="29" t="s">
+      <c r="H43" s="51"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1722,18 +1791,22 @@
       <c r="C44" s="19">
         <v>201</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="27"/>
+      <c r="H44" s="51">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="42"/>
       <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="5">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="28"/>
+      <c r="H45" s="51"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="43"/>
       <c r="B46" s="20" t="s">
         <v>7</v>
       </c>
@@ -1743,9 +1816,10 @@
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="29" t="s">
+      <c r="H46" s="51"/>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -1755,7 +1829,7 @@
         <f>E47+F47</f>
         <v>766</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="45" t="s">
         <v>34</v>
       </c>
       <c r="E47" s="19">
@@ -1764,53 +1838,57 @@
       <c r="F47" s="19">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="27"/>
-      <c r="B48" s="49" t="s">
+      <c r="H47" s="51">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="42"/>
+      <c r="B48" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="42">
+      <c r="C48" s="26">
         <f>127</f>
         <v>127</v>
       </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="42">
+      <c r="D48" s="45"/>
+      <c r="E48" s="26">
         <v>121</v>
       </c>
-      <c r="F48" s="42">
+      <c r="F48" s="26">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="28"/>
-      <c r="B49" s="50" t="s">
+      <c r="H48" s="51"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="43"/>
+      <c r="B49" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="27">
         <v>129</v>
       </c>
-      <c r="D49" s="34"/>
-      <c r="E49" s="43">
+      <c r="D49" s="46"/>
+      <c r="E49" s="27">
         <v>121</v>
       </c>
-      <c r="F49" s="43">
+      <c r="F49" s="27">
         <v>8</v>
       </c>
       <c r="G49" s="22"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="29" t="s">
+      <c r="H49" s="51"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="19" t="e" cm="1">
-        <f t="array" ref="C50">E50+E55F50+G50</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D50" s="35" t="s">
+      <c r="C50" s="19">
+        <v>766</v>
+      </c>
+      <c r="D50" s="47" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="19">
@@ -1822,9 +1900,12 @@
       <c r="G50" s="19">
         <v>71</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="27"/>
+      <c r="H50" s="51">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="42"/>
       <c r="B51" s="4" t="s">
         <v>11</v>
       </c>
@@ -1832,19 +1913,20 @@
         <f>E51+F51+G51</f>
         <v>127</v>
       </c>
-      <c r="D51" s="36"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="5">
         <v>68</v>
       </c>
       <c r="F51" s="5">
         <v>55</v>
       </c>
-      <c r="G51" s="42">
+      <c r="G51" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="28"/>
+      <c r="H51" s="51"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="43"/>
       <c r="B52" s="20" t="s">
         <v>7</v>
       </c>
@@ -1852,19 +1934,20 @@
         <f>E52+F52+G52</f>
         <v>129</v>
       </c>
-      <c r="D52" s="37"/>
+      <c r="D52" s="49"/>
       <c r="E52" s="21">
         <v>57</v>
       </c>
       <c r="F52" s="21">
         <v>65</v>
       </c>
-      <c r="G52" s="43">
+      <c r="G52" s="27">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="29" t="s">
+      <c r="H52" s="51"/>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B53" s="18" t="s">
@@ -1873,41 +1956,66 @@
       <c r="C53" s="11">
         <v>798</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="27"/>
+      <c r="H53" s="51">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="42"/>
       <c r="B54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="12">
         <v>130</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="32"/>
+      <c r="H54" s="51"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="44"/>
       <c r="B55" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="14">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H55" s="51"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D56" s="23"/>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D57" s="24"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D58" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="D26:D28"/>
+  <mergeCells count="42">
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A53:A55"/>
@@ -1920,13 +2028,11 @@
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="A32:A34"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="D26:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished phyloglm UN models
</commit_message>
<xml_diff>
--- a/Notes/Coastal_Sample_Size_Corr.xlsx
+++ b/Notes/Coastal_Sample_Size_Corr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{254FBCFA-0BA0-4808-B627-D30555D4B8E4}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A53A712-0758-4191-B782-D24DE98DAD95}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -438,17 +438,6 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
       <right style="medium">
         <color rgb="FFCCCCCC"/>
       </right>
@@ -520,9 +509,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -581,49 +570,82 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -639,41 +661,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -691,10 +689,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1016,9 +1010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1970122C-29C4-4E46-A235-3E0E6C7793EA}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1060,7 +1054,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1073,7 +1067,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
-      <c r="H2" s="51">
+      <c r="H2" s="35">
         <v>237</v>
       </c>
     </row>
@@ -1089,7 +1083,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="51"/>
+      <c r="H3" s="35"/>
       <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1103,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
-      <c r="H4" s="51"/>
+      <c r="H4" s="35"/>
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1118,7 +1112,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="44" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1131,7 +1125,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="51">
+      <c r="H5" s="35">
         <v>210</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -1153,7 +1147,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="51"/>
+      <c r="H6" s="35"/>
       <c r="K6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1173,10 +1167,10 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="51"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1189,7 +1183,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="51">
+      <c r="H8" s="35">
         <v>807</v>
       </c>
     </row>
@@ -1205,7 +1199,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="51"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="43"/>
@@ -1219,10 +1213,10 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="51"/>
+      <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1235,7 +1229,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="51">
+      <c r="H11" s="35">
         <v>805</v>
       </c>
     </row>
@@ -1251,7 +1245,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="51"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="43"/>
@@ -1265,10 +1259,10 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="51"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:12" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1281,7 +1275,7 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="51">
+      <c r="H14" s="35">
         <v>746</v>
       </c>
     </row>
@@ -1297,7 +1291,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="51"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="43"/>
@@ -1311,10 +1305,10 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="51"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1323,13 +1317,11 @@
       <c r="C17" s="3">
         <v>408</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>23</v>
-      </c>
+      <c r="D17" s="53"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="51">
+      <c r="H17" s="35">
         <v>484</v>
       </c>
     </row>
@@ -1341,11 +1333,11 @@
       <c r="C18" s="5">
         <v>121</v>
       </c>
-      <c r="D18" s="38"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="51"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="43"/>
@@ -1355,14 +1347,14 @@
       <c r="C19" s="7">
         <v>102</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="51"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1371,8 +1363,8 @@
       <c r="C20" s="3">
         <v>766</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>22</v>
+      <c r="D20" s="49" t="s">
+        <v>23</v>
       </c>
       <c r="E20" s="15">
         <v>421</v>
@@ -1381,7 +1373,7 @@
         <v>345</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="51">
+      <c r="H20" s="35">
         <v>775</v>
       </c>
       <c r="I20" t="s">
@@ -1396,7 +1388,7 @@
       <c r="C21" s="5">
         <v>127</v>
       </c>
-      <c r="D21" s="36"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="16">
         <v>73</v>
       </c>
@@ -1404,7 +1396,7 @@
         <v>54</v>
       </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="51"/>
+      <c r="H21" s="35"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="43"/>
@@ -1414,7 +1406,7 @@
       <c r="C22" s="7">
         <v>129</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29">
         <v>97</v>
       </c>
@@ -1422,10 +1414,10 @@
         <v>32</v>
       </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="51"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="44" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1435,8 +1427,8 @@
         <f>E20+F20</f>
         <v>766</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>24</v>
+      <c r="D23" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="E23" s="19">
         <v>118</v>
@@ -1445,7 +1437,7 @@
         <v>615</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="51">
+      <c r="H23" s="35">
         <v>741</v>
       </c>
     </row>
@@ -1457,7 +1449,7 @@
       <c r="C24" s="5">
         <v>117</v>
       </c>
-      <c r="D24" s="38"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="31">
         <v>10</v>
       </c>
@@ -1465,7 +1457,7 @@
         <v>107</v>
       </c>
       <c r="G24" s="17"/>
-      <c r="H24" s="51"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="43"/>
@@ -1475,7 +1467,7 @@
       <c r="C25" s="28">
         <v>122</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="28">
         <v>8</v>
       </c>
@@ -1483,10 +1475,10 @@
         <v>114</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="51"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="44" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1496,8 +1488,8 @@
         <f t="shared" ref="C26:C31" si="0">E23+F23</f>
         <v>733</v>
       </c>
-      <c r="D26" s="40" t="s">
-        <v>27</v>
+      <c r="D26" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="E26" s="3">
         <v>289</v>
@@ -1506,7 +1498,7 @@
         <v>507</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="51">
+      <c r="H26" s="35">
         <v>805</v>
       </c>
     </row>
@@ -1519,7 +1511,7 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="D27" s="38"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="5">
         <v>55</v>
       </c>
@@ -1527,7 +1519,7 @@
         <v>75</v>
       </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="51"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="43"/>
@@ -1538,7 +1530,7 @@
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="D28" s="38"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="7">
         <v>79</v>
       </c>
@@ -1546,10 +1538,10 @@
         <v>50</v>
       </c>
       <c r="G28" s="17"/>
-      <c r="H28" s="51"/>
+      <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="44" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1559,7 +1551,9 @@
         <f t="shared" si="0"/>
         <v>796</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="E29" s="3">
         <v>290</v>
       </c>
@@ -1567,7 +1561,7 @@
         <v>506</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="51">
+      <c r="H29" s="35">
         <v>805</v>
       </c>
     </row>
@@ -1580,7 +1574,7 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="5">
         <v>36</v>
       </c>
@@ -1588,7 +1582,7 @@
         <v>94</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="51"/>
+      <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="43"/>
@@ -1599,7 +1593,7 @@
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="D31" s="17"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="7">
         <v>25</v>
       </c>
@@ -1607,10 +1601,10 @@
         <v>104</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="51"/>
+      <c r="H31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="44" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1623,7 +1617,7 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="51">
+      <c r="H32" s="35">
         <v>775</v>
       </c>
     </row>
@@ -1639,7 +1633,7 @@
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
-      <c r="H33" s="51"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="43"/>
@@ -1653,10 +1647,10 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="51"/>
+      <c r="H34" s="35"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1669,7 +1663,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="51">
+      <c r="H35" s="35">
         <v>775</v>
       </c>
     </row>
@@ -1685,7 +1679,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="51"/>
+      <c r="H36" s="35"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="43"/>
@@ -1699,10 +1693,10 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
-      <c r="H37" s="51"/>
+      <c r="H37" s="35"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -1715,7 +1709,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="51">
+      <c r="H38" s="35">
         <v>775</v>
       </c>
     </row>
@@ -1731,7 +1725,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="51"/>
+      <c r="H39" s="35"/>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="43"/>
@@ -1745,10 +1739,10 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="51"/>
+      <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="18" t="s">
@@ -1757,7 +1751,7 @@
       <c r="C41" s="19">
         <v>201</v>
       </c>
-      <c r="H41" s="51">
+      <c r="H41" s="35">
         <v>202</v>
       </c>
     </row>
@@ -1769,7 +1763,7 @@
       <c r="C42" s="5">
         <v>67</v>
       </c>
-      <c r="H42" s="51"/>
+      <c r="H42" s="35"/>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="43"/>
@@ -1779,10 +1773,10 @@
       <c r="C43" s="21">
         <v>61</v>
       </c>
-      <c r="H43" s="51"/>
+      <c r="H43" s="35"/>
     </row>
     <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="44" t="s">
         <v>32</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1791,7 +1785,7 @@
       <c r="C44" s="19">
         <v>201</v>
       </c>
-      <c r="H44" s="51">
+      <c r="H44" s="35">
         <v>202</v>
       </c>
     </row>
@@ -1803,7 +1797,7 @@
       <c r="C45" s="5">
         <v>67</v>
       </c>
-      <c r="H45" s="51"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="43"/>
@@ -1816,10 +1810,10 @@
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-      <c r="H46" s="51"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -1829,7 +1823,7 @@
         <f>E47+F47</f>
         <v>766</v>
       </c>
-      <c r="D47" s="45" t="s">
+      <c r="D47" s="36" t="s">
         <v>34</v>
       </c>
       <c r="E47" s="19">
@@ -1838,7 +1832,7 @@
       <c r="F47" s="19">
         <v>31</v>
       </c>
-      <c r="H47" s="51">
+      <c r="H47" s="35">
         <v>775</v>
       </c>
     </row>
@@ -1851,14 +1845,14 @@
         <f>127</f>
         <v>127</v>
       </c>
-      <c r="D48" s="45"/>
+      <c r="D48" s="36"/>
       <c r="E48" s="26">
         <v>121</v>
       </c>
       <c r="F48" s="26">
         <v>6</v>
       </c>
-      <c r="H48" s="51"/>
+      <c r="H48" s="35"/>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="43"/>
@@ -1868,7 +1862,7 @@
       <c r="C49" s="27">
         <v>129</v>
       </c>
-      <c r="D49" s="46"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="27">
         <v>121</v>
       </c>
@@ -1876,10 +1870,10 @@
         <v>8</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="51"/>
+      <c r="H49" s="35"/>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="44" t="s">
         <v>35</v>
       </c>
       <c r="B50" s="18" t="s">
@@ -1888,7 +1882,7 @@
       <c r="C50" s="19">
         <v>766</v>
       </c>
-      <c r="D50" s="47" t="s">
+      <c r="D50" s="38" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="19">
@@ -1900,7 +1894,7 @@
       <c r="G50" s="19">
         <v>71</v>
       </c>
-      <c r="H50" s="51">
+      <c r="H50" s="35">
         <v>775</v>
       </c>
     </row>
@@ -1913,7 +1907,7 @@
         <f>E51+F51+G51</f>
         <v>127</v>
       </c>
-      <c r="D51" s="48"/>
+      <c r="D51" s="39"/>
       <c r="E51" s="5">
         <v>68</v>
       </c>
@@ -1923,7 +1917,7 @@
       <c r="G51" s="26">
         <v>4</v>
       </c>
-      <c r="H51" s="51"/>
+      <c r="H51" s="35"/>
     </row>
     <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="43"/>
@@ -1934,7 +1928,7 @@
         <f>E52+F52+G52</f>
         <v>129</v>
       </c>
-      <c r="D52" s="49"/>
+      <c r="D52" s="40"/>
       <c r="E52" s="21">
         <v>57</v>
       </c>
@@ -1944,10 +1938,10 @@
       <c r="G52" s="27">
         <v>7</v>
       </c>
-      <c r="H52" s="51"/>
+      <c r="H52" s="35"/>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B53" s="18" t="s">
@@ -1956,7 +1950,7 @@
       <c r="C53" s="11">
         <v>798</v>
       </c>
-      <c r="H53" s="51">
+      <c r="H53" s="35">
         <v>807</v>
       </c>
     </row>
@@ -1968,17 +1962,17 @@
       <c r="C54" s="12">
         <v>130</v>
       </c>
-      <c r="H54" s="51"/>
+      <c r="H54" s="35"/>
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="44"/>
+      <c r="A55" s="45"/>
       <c r="B55" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="14">
         <v>129</v>
       </c>
-      <c r="H55" s="51"/>
+      <c r="H55" s="35"/>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D56" s="23"/>
@@ -1991,33 +1985,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A53:A55"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A38:A40"/>
@@ -2028,11 +1995,38 @@
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A35:A37"/>
     <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D17:D19"/>
     <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A29:A31"/>
     <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ran Sarah's FIXED phyloglm models (on Emma's computer) and saved model outputs. Recorded values for results.
</commit_message>
<xml_diff>
--- a/Notes/Coastal_Sample_Size_Corr.xlsx
+++ b/Notes/Coastal_Sample_Size_Corr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A53A712-0758-4191-B782-D24DE98DAD95}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{A3946400-3771-4533-A9AB-B304F018401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D385E61-E032-442F-AC9C-569B319A5B5F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{2B7A2C83-8A21-44A0-807B-D4C4840C4DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -613,65 +613,65 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -689,6 +689,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,7 +1016,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,7 +1058,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1067,12 +1071,12 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
-      <c r="H2" s="35">
+      <c r="H2" s="54">
         <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="42"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1087,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="35"/>
+      <c r="H3" s="54"/>
       <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1092,7 +1096,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="43"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1103,7 +1107,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
-      <c r="H4" s="35"/>
+      <c r="H4" s="54"/>
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1112,7 +1116,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1125,7 +1129,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="35">
+      <c r="H5" s="54">
         <v>210</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -1136,7 +1140,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="42"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1151,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="35"/>
+      <c r="H6" s="54"/>
       <c r="K6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1156,7 +1160,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1167,10 +1171,10 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="35"/>
+      <c r="H7" s="54"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="37" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1183,12 +1187,12 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="35">
+      <c r="H8" s="54">
         <v>807</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="42"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1199,10 +1203,10 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="35"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="43"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1213,10 +1217,10 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="35"/>
+      <c r="H10" s="54"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1229,12 +1233,12 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="35">
+      <c r="H11" s="54">
         <v>805</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="42"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1245,10 +1249,10 @@
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="35"/>
+      <c r="H12" s="54"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="43"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
@@ -1259,10 +1263,10 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="35"/>
+      <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:12" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1275,12 +1279,12 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="35">
+      <c r="H14" s="54">
         <v>746</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="42"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1291,10 +1295,10 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="35"/>
+      <c r="H15" s="54"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="43"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1305,10 +1309,10 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="35"/>
+      <c r="H16" s="54"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1317,44 +1321,44 @@
       <c r="C17" s="3">
         <v>408</v>
       </c>
-      <c r="D17" s="53"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="35">
+      <c r="H17" s="54">
         <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="42"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5">
         <v>121</v>
       </c>
-      <c r="D18" s="53"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="35"/>
+      <c r="H18" s="54"/>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7">
         <v>102</v>
       </c>
-      <c r="D19" s="54"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="35"/>
+      <c r="H19" s="54"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1363,7 +1367,7 @@
       <c r="C20" s="3">
         <v>766</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="47" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="15">
@@ -1373,7 +1377,7 @@
         <v>345</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="35">
+      <c r="H20" s="54">
         <v>775</v>
       </c>
       <c r="I20" t="s">
@@ -1381,14 +1385,14 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="42"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>127</v>
       </c>
-      <c r="D21" s="49"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="16">
         <v>73</v>
       </c>
@@ -1396,17 +1400,17 @@
         <v>54</v>
       </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="35"/>
+      <c r="H21" s="54"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="43"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="7">
         <v>129</v>
       </c>
-      <c r="D22" s="50"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="29">
         <v>97</v>
       </c>
@@ -1414,10 +1418,10 @@
         <v>32</v>
       </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="35"/>
+      <c r="H22" s="54"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1427,7 +1431,7 @@
         <f>E20+F20</f>
         <v>766</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="49" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="19">
@@ -1437,19 +1441,19 @@
         <v>615</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="35">
+      <c r="H23" s="54">
         <v>741</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="42"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>117</v>
       </c>
-      <c r="D24" s="47"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="31">
         <v>10</v>
       </c>
@@ -1457,17 +1461,17 @@
         <v>107</v>
       </c>
       <c r="G24" s="17"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="43"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="28">
         <v>122</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="28">
         <v>8</v>
       </c>
@@ -1475,10 +1479,10 @@
         <v>114</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="35"/>
+      <c r="H25" s="54"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1488,7 +1492,7 @@
         <f t="shared" ref="C26:C31" si="0">E23+F23</f>
         <v>733</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="52" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="3">
@@ -1498,12 +1502,12 @@
         <v>507</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="35">
+      <c r="H26" s="54">
         <v>805</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="42"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1515,7 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="5">
         <v>55</v>
       </c>
@@ -1519,10 +1523,10 @@
         <v>75</v>
       </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="35"/>
+      <c r="H27" s="54"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="43"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="6" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1534,7 @@
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="51"/>
       <c r="E28" s="7">
         <v>79</v>
       </c>
@@ -1538,10 +1542,10 @@
         <v>50</v>
       </c>
       <c r="G28" s="17"/>
-      <c r="H28" s="35"/>
+      <c r="H28" s="54"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="37" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1551,7 +1555,7 @@
         <f t="shared" si="0"/>
         <v>796</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="52" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="3">
@@ -1561,12 +1565,12 @@
         <v>506</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="35">
+      <c r="H29" s="54">
         <v>805</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="42"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1574,7 +1578,7 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="5">
         <v>36</v>
       </c>
@@ -1582,10 +1586,10 @@
         <v>94</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="35"/>
+      <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="43"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
@@ -1593,7 +1597,7 @@
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="D31" s="52"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="7">
         <v>25</v>
       </c>
@@ -1601,10 +1605,10 @@
         <v>104</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="35"/>
+      <c r="H31" s="54"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1617,12 +1621,12 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="35">
+      <c r="H32" s="54">
         <v>775</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="42"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
@@ -1633,10 +1637,10 @@
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
-      <c r="H33" s="35"/>
+      <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="43"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
@@ -1647,10 +1651,10 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="35"/>
+      <c r="H34" s="54"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1663,12 +1667,12 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="35">
+      <c r="H35" s="54">
         <v>775</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="42"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
@@ -1679,10 +1683,10 @@
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="35"/>
+      <c r="H36" s="54"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="43"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="20" t="s">
         <v>7</v>
       </c>
@@ -1693,10 +1697,10 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
-      <c r="H37" s="35"/>
+      <c r="H37" s="54"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -1709,12 +1713,12 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="35">
+      <c r="H38" s="54">
         <v>775</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="42"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1725,10 +1729,10 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="35"/>
+      <c r="H39" s="54"/>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="43"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="20" t="s">
         <v>7</v>
       </c>
@@ -1739,10 +1743,10 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="35"/>
+      <c r="H40" s="54"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="18" t="s">
@@ -1751,32 +1755,32 @@
       <c r="C41" s="19">
         <v>201</v>
       </c>
-      <c r="H41" s="35">
+      <c r="H41" s="54">
         <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="42"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="5">
         <v>67</v>
       </c>
-      <c r="H42" s="35"/>
+      <c r="H42" s="54"/>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="43"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="21">
         <v>61</v>
       </c>
-      <c r="H43" s="35"/>
+      <c r="H43" s="54"/>
     </row>
     <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="37" t="s">
         <v>32</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1785,22 +1789,22 @@
       <c r="C44" s="19">
         <v>201</v>
       </c>
-      <c r="H44" s="35">
+      <c r="H44" s="54">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="42"/>
+      <c r="A45" s="38"/>
       <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="5">
         <v>67</v>
       </c>
-      <c r="H45" s="35"/>
+      <c r="H45" s="54"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="43"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="20" t="s">
         <v>7</v>
       </c>
@@ -1810,10 +1814,10 @@
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-      <c r="H46" s="35"/>
+      <c r="H46" s="54"/>
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -1823,7 +1827,7 @@
         <f>E47+F47</f>
         <v>766</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E47" s="19">
@@ -1832,12 +1836,12 @@
       <c r="F47" s="19">
         <v>31</v>
       </c>
-      <c r="H47" s="35">
+      <c r="H47" s="54">
         <v>775</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="32" t="s">
         <v>11</v>
       </c>
@@ -1845,24 +1849,24 @@
         <f>127</f>
         <v>127</v>
       </c>
-      <c r="D48" s="36"/>
+      <c r="D48" s="41"/>
       <c r="E48" s="26">
         <v>121</v>
       </c>
       <c r="F48" s="26">
         <v>6</v>
       </c>
-      <c r="H48" s="35"/>
+      <c r="H48" s="54"/>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="43"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="27">
         <v>129</v>
       </c>
-      <c r="D49" s="37"/>
+      <c r="D49" s="42"/>
       <c r="E49" s="27">
         <v>121</v>
       </c>
@@ -1870,10 +1874,10 @@
         <v>8</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="35"/>
+      <c r="H49" s="54"/>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="37" t="s">
         <v>35</v>
       </c>
       <c r="B50" s="18" t="s">
@@ -1882,7 +1886,7 @@
       <c r="C50" s="19">
         <v>766</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="43" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="19">
@@ -1894,12 +1898,12 @@
       <c r="G50" s="19">
         <v>71</v>
       </c>
-      <c r="H50" s="35">
+      <c r="H50" s="54">
         <v>775</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="42"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="4" t="s">
         <v>11</v>
       </c>
@@ -1907,7 +1911,7 @@
         <f>E51+F51+G51</f>
         <v>127</v>
       </c>
-      <c r="D51" s="39"/>
+      <c r="D51" s="44"/>
       <c r="E51" s="5">
         <v>68</v>
       </c>
@@ -1917,10 +1921,10 @@
       <c r="G51" s="26">
         <v>4</v>
       </c>
-      <c r="H51" s="35"/>
+      <c r="H51" s="54"/>
     </row>
     <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="43"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="20" t="s">
         <v>7</v>
       </c>
@@ -1928,7 +1932,7 @@
         <f>E52+F52+G52</f>
         <v>129</v>
       </c>
-      <c r="D52" s="40"/>
+      <c r="D52" s="45"/>
       <c r="E52" s="21">
         <v>57</v>
       </c>
@@ -1938,10 +1942,10 @@
       <c r="G52" s="27">
         <v>7</v>
       </c>
-      <c r="H52" s="35"/>
+      <c r="H52" s="54"/>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B53" s="18" t="s">
@@ -1950,29 +1954,29 @@
       <c r="C53" s="11">
         <v>798</v>
       </c>
-      <c r="H53" s="35">
+      <c r="H53" s="54">
         <v>807</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="42"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="12">
         <v>130</v>
       </c>
-      <c r="H54" s="35"/>
+      <c r="H54" s="54"/>
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="45"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="14">
         <v>129</v>
       </c>
-      <c r="H55" s="35"/>
+      <c r="H55" s="54"/>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D56" s="23"/>
@@ -1985,17 +1989,24 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H16"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="D50:D52"/>
     <mergeCell ref="A2:A4"/>
@@ -2009,24 +2020,17 @@
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="D29:D31"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A29:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>